<commit_message>
hosteller logic updated for report
</commit_message>
<xml_diff>
--- a/backend/reports/Boys_Absent_Students_2024-12-18.xlsx
+++ b/backend/reports/Boys_Absent_Students_2024-12-18.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Kongu Engineering College</t>
   </si>
@@ -37,22 +37,16 @@
     <t>Branch</t>
   </si>
   <si>
-    <t>22ALR052</t>
-  </si>
-  <si>
-    <t>MOHAMMED RIFATH J</t>
+    <t>22ALR056</t>
+  </si>
+  <si>
+    <t>NAVEEN SAKTHI S</t>
   </si>
   <si>
     <t>III</t>
   </si>
   <si>
     <t>AIML-A</t>
-  </si>
-  <si>
-    <t>22ALR056</t>
-  </si>
-  <si>
-    <t>NAVEEN SAKTHI S</t>
   </si>
 </sst>
 </file>
@@ -454,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -484,7 +478,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -515,23 +509,6 @@
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" ht="25" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>